<commit_message>
Update to WP4 data dictionary
1_1_monthly_rep: hba1c units changed to %. Information category labels for heightmes_ and weightmes_added in the categories tab. 
1_1_weekly_rep: hba1c units changed to %
1_1_non_rep: hba1c units changed to %
</commit_message>
<xml_diff>
--- a/R/data/dictionaries/outcome/1_1/1_1_non_rep.xlsx
+++ b/R/data/dictionaries/outcome/1_1/1_1_non_rep.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/RProjects/analysis-protocols/R/data/dictionaries/outcome/1_0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/ae16175_bristol_ac_uk/Documents/MyFiles-Migrated/LifeCycle/wp4_data_dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7126A91C-43C3-8C47-BAA6-A6856229D8A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{7126A91C-43C3-8C47-BAA6-A6856229D8A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1BD60C05-4FD5-4371-AFF7-17D5DFF743EC}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
     <sheet name="Categories" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="91">
   <si>
     <t>name</t>
   </si>
@@ -291,6 +292,9 @@
   </si>
   <si>
     <t>pets_preg</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
@@ -901,19 +905,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BG39"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" style="1" customWidth="1"/>
-    <col min="2" max="3" width="15.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="74.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="20.36328125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="15.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="74.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -982,7 +986,7 @@
       <c r="BF1"/>
       <c r="BG1"/>
     </row>
-    <row r="2" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>33</v>
       </c>
@@ -996,7 +1000,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>37</v>
       </c>
@@ -1008,7 +1012,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>5</v>
       </c>
@@ -1023,7 +1027,7 @@
       </c>
       <c r="E4"/>
     </row>
-    <row r="5" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
@@ -1038,7 +1042,7 @@
       </c>
       <c r="E5"/>
     </row>
-    <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>7</v>
       </c>
@@ -1046,14 +1050,14 @@
         <v>4</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>21</v>
       </c>
       <c r="E6"/>
     </row>
-    <row r="7" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>8</v>
       </c>
@@ -1068,7 +1072,7 @@
       </c>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>9</v>
       </c>
@@ -1083,7 +1087,7 @@
       </c>
       <c r="E8"/>
     </row>
-    <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
         <v>10</v>
       </c>
@@ -1098,7 +1102,7 @@
       </c>
       <c r="E9"/>
     </row>
-    <row r="10" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>11</v>
       </c>
@@ -1113,7 +1117,7 @@
       </c>
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
         <v>12</v>
       </c>
@@ -1128,7 +1132,7 @@
       </c>
       <c r="E11"/>
     </row>
-    <row r="12" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
         <v>13</v>
       </c>
@@ -1143,7 +1147,7 @@
       </c>
       <c r="E12"/>
     </row>
-    <row r="13" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
         <v>14</v>
       </c>
@@ -1158,7 +1162,7 @@
       </c>
       <c r="E13"/>
     </row>
-    <row r="14" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>15</v>
       </c>
@@ -1173,7 +1177,7 @@
       </c>
       <c r="E14"/>
     </row>
-    <row r="15" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
         <v>16</v>
       </c>
@@ -1188,7 +1192,7 @@
       </c>
       <c r="E15"/>
     </row>
-    <row r="16" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:59" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
         <v>17</v>
       </c>
@@ -1203,7 +1207,7 @@
       </c>
       <c r="E16"/>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
         <v>41</v>
       </c>
@@ -1215,7 +1219,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>43</v>
       </c>
@@ -1227,7 +1231,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>45</v>
       </c>
@@ -1239,7 +1243,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="11" t="s">
         <v>47</v>
       </c>
@@ -1251,7 +1255,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
         <v>49</v>
       </c>
@@ -1263,7 +1267,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
         <v>51</v>
       </c>
@@ -1275,7 +1279,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
         <v>53</v>
       </c>
@@ -1287,7 +1291,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
         <v>55</v>
       </c>
@@ -1299,7 +1303,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
         <v>57</v>
       </c>
@@ -1311,7 +1315,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
         <v>59</v>
       </c>
@@ -1323,7 +1327,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
         <v>61</v>
       </c>
@@ -1335,7 +1339,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
         <v>88</v>
       </c>
@@ -1347,7 +1351,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
         <v>64</v>
       </c>
@@ -1359,7 +1363,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
         <v>66</v>
       </c>
@@ -1371,7 +1375,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
         <v>68</v>
       </c>
@@ -1383,7 +1387,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
         <v>70</v>
       </c>
@@ -1395,7 +1399,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
         <v>72</v>
       </c>
@@ -1407,7 +1411,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
         <v>74</v>
       </c>
@@ -1419,7 +1423,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
         <v>76</v>
       </c>
@@ -1431,7 +1435,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
         <v>78</v>
       </c>
@@ -1443,7 +1447,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
         <v>80</v>
       </c>
@@ -1455,7 +1459,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="11" t="s">
         <v>82</v>
       </c>
@@ -1467,7 +1471,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="11" t="s">
         <v>89</v>
       </c>
@@ -1493,18 +1497,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="55.5" style="1" customWidth="1"/>
-    <col min="2" max="4" width="14.1640625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="1"/>
+    <col min="1" max="1" width="55.453125" style="1" customWidth="1"/>
+    <col min="2" max="4" width="14.1796875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
@@ -1518,7 +1522,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>41</v>
       </c>
@@ -1532,7 +1536,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
@@ -1546,7 +1550,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>43</v>
       </c>
@@ -1560,7 +1564,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>43</v>
       </c>
@@ -1574,7 +1578,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>45</v>
       </c>
@@ -1588,7 +1592,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>45</v>
       </c>
@@ -1602,7 +1606,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>47</v>
       </c>
@@ -1616,7 +1620,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>47</v>
       </c>
@@ -1630,7 +1634,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>49</v>
       </c>
@@ -1644,7 +1648,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>49</v>
       </c>
@@ -1658,7 +1662,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -1672,7 +1676,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -1686,7 +1690,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>53</v>
       </c>
@@ -1700,7 +1704,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>53</v>
       </c>
@@ -1714,7 +1718,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>55</v>
       </c>
@@ -1728,7 +1732,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>55</v>
       </c>
@@ -1742,7 +1746,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>57</v>
       </c>
@@ -1756,7 +1760,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>57</v>
       </c>
@@ -1770,7 +1774,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>59</v>
       </c>
@@ -1784,7 +1788,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>59</v>
       </c>
@@ -1798,7 +1802,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>61</v>
       </c>
@@ -1812,7 +1816,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>61</v>
       </c>
@@ -1826,7 +1830,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>88</v>
       </c>
@@ -1840,7 +1844,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>88</v>
       </c>
@@ -1854,7 +1858,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>64</v>
       </c>
@@ -1868,7 +1872,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>64</v>
       </c>
@@ -1882,7 +1886,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
         <v>66</v>
       </c>
@@ -1896,7 +1900,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
         <v>66</v>
       </c>
@@ -1910,7 +1914,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>68</v>
       </c>
@@ -1924,7 +1928,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>68</v>
       </c>
@@ -1938,7 +1942,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
         <v>70</v>
       </c>
@@ -1952,7 +1956,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
         <v>70</v>
       </c>
@@ -1966,7 +1970,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
         <v>72</v>
       </c>
@@ -1980,7 +1984,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
         <v>72</v>
       </c>
@@ -1994,7 +1998,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
         <v>74</v>
       </c>
@@ -2008,7 +2012,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
         <v>74</v>
       </c>
@@ -2022,7 +2026,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>76</v>
       </c>
@@ -2036,7 +2040,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>76</v>
       </c>
@@ -2050,7 +2054,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>78</v>
       </c>
@@ -2064,7 +2068,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
         <v>78</v>
       </c>
@@ -2078,7 +2082,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4" t="s">
         <v>80</v>
       </c>
@@ -2092,7 +2096,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>80</v>
       </c>
@@ -2106,7 +2110,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
         <v>82</v>
       </c>
@@ -2120,7 +2124,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
         <v>82</v>
       </c>
@@ -2134,7 +2138,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4" t="s">
         <v>89</v>
       </c>
@@ -2148,7 +2152,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
         <v>89</v>
       </c>

</xml_diff>